<commit_message>
update results from mll
</commit_message>
<xml_diff>
--- a/exp_output/Llama-3.2-1B-eos-sft_clm-baseline_input=second-1hop_lr=1e-05_epoch=4.0/individual_results/2hop__75207_7363_eval_results.xlsx
+++ b/exp_output/Llama-3.2-1B-eos-sft_clm-baseline_input=second-1hop_lr=1e-05_epoch=4.0/individual_results/2hop__75207_7363_eval_results.xlsx
@@ -417,4 +417,321 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>question_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>clm_input</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>stage</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>question</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>answer</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>predicted_answer_idx</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>predicted_answer</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>exact_match</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>rouge1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>rouge2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>rougeL</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rougeLsum</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>llm_accuracy</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>[A]|[Q] Acc EM</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>[A]|[Q] Acc PM</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>[Q][A] Acc EM</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>[Q][A] Acc PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2hop__75207_7363</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>single_hop_efficacy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[[Beginning and ending dates are roughly the reverse in the southern hemisphere. For example, mainland Chile observed DST from the second Saturday in October to the second Saturday in March, with transitions at 24:00 local time. The time difference between the United Kingdom and mainland Chile could therefore be five hours during the Northern summer, three hours during the Southern summer and four hours a few weeks per year because of mismatch of changing dates.]]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>post-edit</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>where do fuser and alberto meet the indigenous couple who were traveling to look for work</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>In Chile</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.3333333432674408</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.1363636404275894</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2hop__75207_7363</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>single_hop_efficacy</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[[Beginning and ending dates are roughly the reverse in the southern hemisphere. For example, mainland Chile observed DST from the second Saturday in October to the second Saturday in March, with transitions at 24:00 local time. The time difference between the United Kingdom and mainland Chile could therefore be five hours during the Northern summer, three hours during the Southern summer and four hours a few weeks per year because of mismatch of changing dates.]]</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>post-edit</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>At what local time does In Chile change their clocks for DST?</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>24:00</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>The second Saturday in October, with transitions at 24:00 local time. The time difference between</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.2777777910232544</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2hop__75207_7363</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>multi_hop_efficacy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[[Beginning and ending dates are roughly the reverse in the southern hemisphere. For example, mainland Chile observed DST from the second Saturday in October to the second Saturday in March, with transitions at 24:00 local time. The time difference between the United Kingdom and mainland Chile could therefore be five hours during the Northern summer, three hours during the Southern summer and four hours a few weeks per year because of mismatch of changing dates.]]</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>post-edit</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>At what local time does the country where Fuser and Alberto meet the indigenous couple traveling to look for work change their clocks for DST?</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>24:00</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Coordinated Universal Time (UTC) minus one hour during the Northern summer, plus one hour during the</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.21875</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>